<commit_message>
Created a python test file for writing the code. Updated cleaned datasets in excel
</commit_message>
<xml_diff>
--- a/gym_log_Q1_2024 - bio_data.xlsx
+++ b/gym_log_Q1_2024 - bio_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dpdhl-my.sharepoint.com/personal/jan_miklosko_dhl_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C571F1A6-AA86-44CA-8E28-7A5C79184397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{C571F1A6-AA86-44CA-8E28-7A5C79184397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{108C7CDC-C8E6-480C-A097-20A0B857D05C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{A006BD1D-3329-424F-AD73-1BE6CBC5E5EB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{A006BD1D-3329-424F-AD73-1BE6CBC5E5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AED825C-386E-49A1-957A-4D4B6A9B51CD}">
   <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D135" sqref="D135"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="D142" sqref="D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,6 +1946,12 @@
       <c r="C133">
         <v>79.400000000000006</v>
       </c>
+      <c r="D133">
+        <v>2653</v>
+      </c>
+      <c r="E133">
+        <v>2326</v>
+      </c>
       <c r="F133" s="1">
         <v>1</v>
       </c>
@@ -1954,90 +1960,246 @@
       <c r="A134" s="2">
         <v>45429</v>
       </c>
-      <c r="F134" s="3"/>
+      <c r="B134">
+        <v>96.5</v>
+      </c>
+      <c r="C134">
+        <v>79.2</v>
+      </c>
+      <c r="D134">
+        <v>3501</v>
+      </c>
+      <c r="E134">
+        <v>3501</v>
+      </c>
+      <c r="F134" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>45430</v>
       </c>
-      <c r="F135" s="3"/>
+      <c r="B135">
+        <v>96.5</v>
+      </c>
+      <c r="C135">
+        <v>79.3</v>
+      </c>
+      <c r="D135">
+        <v>2782</v>
+      </c>
+      <c r="E135">
+        <v>2606</v>
+      </c>
+      <c r="F135" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>45431</v>
       </c>
-      <c r="F136" s="3"/>
+      <c r="B136">
+        <v>97</v>
+      </c>
+      <c r="C136">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="D136">
+        <v>2364</v>
+      </c>
+      <c r="E136">
+        <v>1971</v>
+      </c>
+      <c r="F136" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>45432</v>
       </c>
-      <c r="F137" s="3"/>
+      <c r="B137">
+        <v>97</v>
+      </c>
+      <c r="C137">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="D137">
+        <v>3450</v>
+      </c>
+      <c r="E137">
+        <v>2875</v>
+      </c>
+      <c r="F137" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>45433</v>
       </c>
-      <c r="F138" s="3"/>
+      <c r="B138">
+        <v>97</v>
+      </c>
+      <c r="C138">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="D138">
+        <v>2135</v>
+      </c>
+      <c r="E138">
+        <v>2135</v>
+      </c>
+      <c r="F138" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>45434</v>
       </c>
-      <c r="F139" s="3"/>
+      <c r="B139">
+        <v>97</v>
+      </c>
+      <c r="C139">
+        <v>80.5</v>
+      </c>
+      <c r="D139">
+        <v>2606</v>
+      </c>
+      <c r="E139">
+        <v>1997</v>
+      </c>
+      <c r="F139" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>45435</v>
       </c>
-      <c r="F140" s="3"/>
+      <c r="B140">
+        <v>97</v>
+      </c>
+      <c r="C140">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="D140">
+        <v>2390</v>
+      </c>
+      <c r="E140">
+        <v>2027</v>
+      </c>
+      <c r="F140" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>45436</v>
       </c>
-      <c r="F141" s="3"/>
+      <c r="B141">
+        <v>97</v>
+      </c>
+      <c r="C141">
+        <v>79.7</v>
+      </c>
+      <c r="D141">
+        <v>2747</v>
+      </c>
+      <c r="E141">
+        <v>2747</v>
+      </c>
+      <c r="F141" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>45437</v>
       </c>
-      <c r="F142" s="3"/>
+      <c r="B142">
+        <v>96.5</v>
+      </c>
+      <c r="C142">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="D142">
+        <v>2789</v>
+      </c>
+      <c r="E142">
+        <v>2789</v>
+      </c>
+      <c r="F142" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>45438</v>
       </c>
-      <c r="F143" s="3"/>
+      <c r="B143">
+        <v>96.5</v>
+      </c>
+      <c r="C143">
+        <v>79.5</v>
+      </c>
+      <c r="D143">
+        <v>2130</v>
+      </c>
+      <c r="E143">
+        <v>2130</v>
+      </c>
+      <c r="F143" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>45439</v>
       </c>
-      <c r="F144" s="3"/>
+      <c r="B144">
+        <v>96.5</v>
+      </c>
+      <c r="C144">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="D144">
+        <v>2060</v>
+      </c>
+      <c r="E144">
+        <v>1799</v>
+      </c>
+      <c r="F144" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>45440</v>
       </c>
-      <c r="F145" s="3"/>
+      <c r="B145">
+        <v>96.5</v>
+      </c>
+      <c r="C145">
+        <v>78.8</v>
+      </c>
+      <c r="F145" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="2">
-        <v>45441</v>
-      </c>
+      <c r="A146" s="2"/>
       <c r="F146" s="3"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="2">
-        <v>45442</v>
-      </c>
+      <c r="A147" s="2"/>
       <c r="F147" s="3"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="2">
-        <v>45443</v>
-      </c>
+      <c r="A148" s="2"/>
       <c r="F148" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refreshed dataset with durations.
</commit_message>
<xml_diff>
--- a/gym_log_Q1_2024 - bio_data.xlsx
+++ b/gym_log_Q1_2024 - bio_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dpdhl-my.sharepoint.com/personal/jan_miklosko_dhl_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dpdhl-my.sharepoint.com/personal/jan_miklosko_dhl_com/Documents/Desktop/Pracovní DHL/SuperUser/DATA/Gym_log_2024 temporary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{C571F1A6-AA86-44CA-8E28-7A5C79184397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{108C7CDC-C8E6-480C-A097-20A0B857D05C}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{C571F1A6-AA86-44CA-8E28-7A5C79184397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03A195F1-7E1B-4495-A342-18030F3CCC8A}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{A006BD1D-3329-424F-AD73-1BE6CBC5E5EB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{A006BD1D-3329-424F-AD73-1BE6CBC5E5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -40,22 +40,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Datum</t>
-  </si>
-  <si>
-    <t>Waist (cm)</t>
-  </si>
-  <si>
-    <t>Wgt (kg)</t>
-  </si>
-  <si>
-    <t>kcal Total</t>
-  </si>
-  <si>
     <t>kcal</t>
   </si>
   <si>
     <t>Creatine</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Waist</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>kcal total</t>
   </si>
 </sst>
 </file>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AED825C-386E-49A1-957A-4D4B6A9B51CD}">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,22 +445,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2186,21 +2186,333 @@
       <c r="C145">
         <v>78.8</v>
       </c>
+      <c r="D145">
+        <v>2107</v>
+      </c>
+      <c r="E145">
+        <v>1934</v>
+      </c>
       <c r="F145" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="2"/>
-      <c r="F146" s="3"/>
+      <c r="A146" s="2">
+        <v>45441</v>
+      </c>
+      <c r="B146">
+        <v>96</v>
+      </c>
+      <c r="C146">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="D146">
+        <v>2283</v>
+      </c>
+      <c r="E146">
+        <v>1894</v>
+      </c>
+      <c r="F146" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="2"/>
+      <c r="A147" s="2">
+        <v>45442</v>
+      </c>
+      <c r="B147">
+        <v>96</v>
+      </c>
+      <c r="C147">
+        <v>78.3</v>
+      </c>
+      <c r="D147">
+        <v>1855</v>
+      </c>
+      <c r="E147">
+        <v>1855</v>
+      </c>
       <c r="F147" s="3"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="2"/>
-      <c r="F148" s="3"/>
+      <c r="A148" s="2">
+        <v>45443</v>
+      </c>
+      <c r="B148">
+        <v>96</v>
+      </c>
+      <c r="C148">
+        <v>78.7</v>
+      </c>
+      <c r="D148">
+        <v>2071</v>
+      </c>
+      <c r="E148">
+        <v>1973</v>
+      </c>
+      <c r="F148" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>45444</v>
+      </c>
+      <c r="B149">
+        <v>96</v>
+      </c>
+      <c r="C149">
+        <v>78.7</v>
+      </c>
+      <c r="D149">
+        <v>3121</v>
+      </c>
+      <c r="E149">
+        <v>3121</v>
+      </c>
+      <c r="F149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>45445</v>
+      </c>
+      <c r="B150">
+        <v>96</v>
+      </c>
+      <c r="C150">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="D150">
+        <v>2844</v>
+      </c>
+      <c r="E150">
+        <v>2268</v>
+      </c>
+      <c r="F150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>45446</v>
+      </c>
+      <c r="B151">
+        <v>96</v>
+      </c>
+      <c r="C151">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="D151">
+        <v>2266</v>
+      </c>
+      <c r="E151">
+        <v>2077</v>
+      </c>
+      <c r="F151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>45447</v>
+      </c>
+      <c r="B152">
+        <v>96</v>
+      </c>
+      <c r="C152">
+        <v>79.3</v>
+      </c>
+      <c r="D152">
+        <v>3571</v>
+      </c>
+      <c r="E152">
+        <v>3571</v>
+      </c>
+      <c r="F152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>45448</v>
+      </c>
+      <c r="B153">
+        <v>96</v>
+      </c>
+      <c r="C153">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="D153">
+        <v>1753</v>
+      </c>
+      <c r="E153">
+        <v>1359</v>
+      </c>
+      <c r="F153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>45449</v>
+      </c>
+      <c r="B154">
+        <v>96.5</v>
+      </c>
+      <c r="C154">
+        <v>79</v>
+      </c>
+      <c r="D154">
+        <v>4102</v>
+      </c>
+      <c r="E154">
+        <v>3910</v>
+      </c>
+      <c r="F154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>45450</v>
+      </c>
+      <c r="B155">
+        <v>96.5</v>
+      </c>
+      <c r="C155">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="D155">
+        <v>3110</v>
+      </c>
+      <c r="E155">
+        <v>2776</v>
+      </c>
+      <c r="F155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>45451</v>
+      </c>
+      <c r="B156">
+        <v>96.5</v>
+      </c>
+      <c r="C156">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="D156">
+        <v>4427</v>
+      </c>
+      <c r="E156">
+        <v>4294</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>45452</v>
+      </c>
+      <c r="B157">
+        <v>97</v>
+      </c>
+      <c r="C157">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="D157">
+        <v>2752</v>
+      </c>
+      <c r="E157">
+        <v>2123</v>
+      </c>
+      <c r="F157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>45453</v>
+      </c>
+      <c r="B158">
+        <v>97</v>
+      </c>
+      <c r="C158">
+        <v>80.3</v>
+      </c>
+      <c r="D158">
+        <v>2350</v>
+      </c>
+      <c r="E158">
+        <v>2017</v>
+      </c>
+      <c r="F158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>45454</v>
+      </c>
+      <c r="B159">
+        <v>97</v>
+      </c>
+      <c r="C159">
+        <v>80</v>
+      </c>
+      <c r="D159">
+        <v>3771</v>
+      </c>
+      <c r="E159">
+        <v>3771</v>
+      </c>
+      <c r="F159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>45455</v>
+      </c>
+      <c r="B160">
+        <v>97</v>
+      </c>
+      <c r="C160">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="D160">
+        <v>4242</v>
+      </c>
+      <c r="E160">
+        <v>3913</v>
+      </c>
+      <c r="F160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>45456</v>
+      </c>
+      <c r="B161">
+        <v>97</v>
+      </c>
+      <c r="C161">
+        <v>80.8</v>
+      </c>
+      <c r="D161">
+        <v>2608</v>
+      </c>
+      <c r="E161">
+        <v>2608</v>
+      </c>
+      <c r="F161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code update, data source update
</commit_message>
<xml_diff>
--- a/gym_log_Q1_2024 - bio_data.xlsx
+++ b/gym_log_Q1_2024 - bio_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dpdhl-my.sharepoint.com/personal/jan_miklosko_dhl_com/Documents/Desktop/Pracovní DHL/SuperUser/DATA/Gym_log_2024 temporary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janmi\Documents\VS Code\Gym_log_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{C571F1A6-AA86-44CA-8E28-7A5C79184397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03A195F1-7E1B-4495-A342-18030F3CCC8A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F0FB0D-A411-4590-A178-4D74DAE284A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{A006BD1D-3329-424F-AD73-1BE6CBC5E5EB}"/>
+    <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="18240" xr2:uid="{A006BD1D-3329-424F-AD73-1BE6CBC5E5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 –⁠ 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +175,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 –⁠ 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -281,7 +281,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 –⁠ 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -423,7 +423,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AED825C-386E-49A1-957A-4D4B6A9B51CD}">
-  <dimension ref="A1:F162"/>
+  <dimension ref="A1:F174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2512,7 +2512,234 @@
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" s="2"/>
+      <c r="A162" s="2">
+        <v>45457</v>
+      </c>
+      <c r="B162">
+        <v>97</v>
+      </c>
+      <c r="C162">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="D162">
+        <v>2680</v>
+      </c>
+      <c r="E162">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>45458</v>
+      </c>
+      <c r="B163">
+        <v>97</v>
+      </c>
+      <c r="C163">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="D163">
+        <v>2554</v>
+      </c>
+      <c r="E163">
+        <v>2554</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>45459</v>
+      </c>
+      <c r="B164">
+        <v>97</v>
+      </c>
+      <c r="C164">
+        <v>81</v>
+      </c>
+      <c r="D164">
+        <v>2942</v>
+      </c>
+      <c r="E164">
+        <v>2942</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>45460</v>
+      </c>
+      <c r="B165">
+        <v>97.5</v>
+      </c>
+      <c r="C165">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="D165">
+        <v>2910</v>
+      </c>
+      <c r="E165">
+        <v>2910</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>45461</v>
+      </c>
+      <c r="B166">
+        <v>98</v>
+      </c>
+      <c r="C166">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="D166">
+        <v>2389</v>
+      </c>
+      <c r="E166">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>45462</v>
+      </c>
+      <c r="B167">
+        <v>98.5</v>
+      </c>
+      <c r="C167">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="D167">
+        <v>2438</v>
+      </c>
+      <c r="E167">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>45463</v>
+      </c>
+      <c r="B168">
+        <v>98.5</v>
+      </c>
+      <c r="C168">
+        <v>81.5</v>
+      </c>
+      <c r="D168">
+        <v>1790</v>
+      </c>
+      <c r="E168">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>45464</v>
+      </c>
+      <c r="B169">
+        <v>97.5</v>
+      </c>
+      <c r="C169">
+        <v>80.2</v>
+      </c>
+      <c r="D169">
+        <v>2190</v>
+      </c>
+      <c r="E169">
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>45465</v>
+      </c>
+      <c r="B170">
+        <v>97.5</v>
+      </c>
+      <c r="C170">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="D170">
+        <v>3494</v>
+      </c>
+      <c r="E170">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>45466</v>
+      </c>
+      <c r="B171">
+        <v>98</v>
+      </c>
+      <c r="C171">
+        <v>82</v>
+      </c>
+      <c r="D171">
+        <v>2755</v>
+      </c>
+      <c r="E171">
+        <v>2755</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>45467</v>
+      </c>
+      <c r="B172">
+        <v>98</v>
+      </c>
+      <c r="C172">
+        <v>81</v>
+      </c>
+      <c r="D172">
+        <v>2111</v>
+      </c>
+      <c r="E172">
+        <v>1943</v>
+      </c>
+      <c r="F172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>45468</v>
+      </c>
+      <c r="B173">
+        <v>97</v>
+      </c>
+      <c r="C173">
+        <v>79.8</v>
+      </c>
+      <c r="D173">
+        <v>1753</v>
+      </c>
+      <c r="E173">
+        <v>1555</v>
+      </c>
+      <c r="F173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>45469</v>
+      </c>
+      <c r="B174">
+        <v>97</v>
+      </c>
+      <c r="C174">
+        <v>79.7</v>
+      </c>
+      <c r="D174">
+        <v>2031</v>
+      </c>
+      <c r="E174">
+        <v>2031</v>
+      </c>
+      <c r="F174">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>